<commit_message>
at bats out of order, nan values on mph when empty
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -1446,7 +1446,7 @@
       </c>
       <c r="J16" s="40" t="inlineStr">
         <is>
-          <t>84-86</t>
+          <t>84-86 MPH</t>
         </is>
       </c>
       <c r="K16" s="34" t="inlineStr">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="J17" s="46" t="inlineStr">
         <is>
-          <t>Fastball,ChangeUp,Slider</t>
+          <t>SL,FB,CH</t>
         </is>
       </c>
       <c r="K17" s="97" t="n"/>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="J25" s="40" t="inlineStr">
         <is>
-          <t>84-84</t>
+          <t>84-84 MPH</t>
         </is>
       </c>
       <c r="K25" s="34" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="J26" s="46" t="inlineStr">
         <is>
-          <t>Fastball,ChangeUp,Slider</t>
+          <t>SL,FB,CH</t>
         </is>
       </c>
       <c r="K26" s="97" t="n"/>

</xml_diff>

<commit_message>
getting closer on postgame hitter
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -1304,11 +1304,7 @@
         </is>
       </c>
       <c r="L10" s="84" t="n"/>
-      <c r="M10" s="52" t="inlineStr">
-        <is>
-          <t>75.42 MPH</t>
-        </is>
-      </c>
+      <c r="M10" s="52" t="inlineStr"/>
       <c r="N10" s="87" t="n"/>
     </row>
     <row r="11">
@@ -1351,11 +1347,7 @@
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M12" s="54" t="inlineStr">
-        <is>
-          <t>14.57°</t>
-        </is>
-      </c>
+      <c r="M12" s="54" t="inlineStr"/>
       <c r="N12" s="93" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1" thickBot="1">
@@ -1542,11 +1534,7 @@
         </is>
       </c>
       <c r="L19" s="84" t="n"/>
-      <c r="M19" s="52" t="inlineStr">
-        <is>
-          <t>61.48 MPH</t>
-        </is>
-      </c>
+      <c r="M19" s="52" t="inlineStr"/>
       <c r="N19" s="87" t="n"/>
     </row>
     <row r="20" ht="14.5" customHeight="1">
@@ -1589,11 +1577,7 @@
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M21" s="54" t="inlineStr">
-        <is>
-          <t>14.14°</t>
-        </is>
-      </c>
+      <c r="M21" s="54" t="inlineStr"/>
       <c r="N21" s="93" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
just need to create strikezone visual for hitters
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -1287,9 +1287,21 @@
       <c r="C10" s="2" t="n"/>
       <c r="D10" s="3" t="n"/>
       <c r="E10" s="3" t="n"/>
-      <c r="F10" s="57" t="n"/>
-      <c r="G10" s="57" t="n"/>
-      <c r="H10" s="36" t="n"/>
+      <c r="F10" s="57" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="G10" s="57" t="inlineStr">
+        <is>
+          <t>Take</t>
+        </is>
+      </c>
+      <c r="H10" s="36" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
       <c r="I10" s="60" t="inlineStr">
         <is>
           <t>Inning:</t>
@@ -1304,16 +1316,32 @@
         </is>
       </c>
       <c r="L10" s="84" t="n"/>
-      <c r="M10" s="52" t="inlineStr"/>
+      <c r="M10" s="52" t="inlineStr">
+        <is>
+          <t>75.42 MPH</t>
+        </is>
+      </c>
       <c r="N10" s="87" t="n"/>
     </row>
     <row r="11">
       <c r="C11" s="4" t="n"/>
       <c r="D11" s="23" t="n"/>
       <c r="E11" s="23" t="n"/>
-      <c r="F11" s="58" t="n"/>
-      <c r="G11" s="58" t="n"/>
-      <c r="H11" s="37" t="n"/>
+      <c r="F11" s="58" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="G11" s="58" t="inlineStr">
+        <is>
+          <t>Swing</t>
+        </is>
+      </c>
+      <c r="H11" s="37" t="inlineStr">
+        <is>
+          <t>Foul</t>
+        </is>
+      </c>
       <c r="I11" s="48" t="inlineStr">
         <is>
           <t>Outs:</t>
@@ -1329,9 +1357,21 @@
       <c r="C12" s="4" t="n"/>
       <c r="D12" s="23" t="n"/>
       <c r="E12" s="23" t="n"/>
-      <c r="F12" s="58" t="n"/>
-      <c r="G12" s="58" t="n"/>
-      <c r="H12" s="37" t="n"/>
+      <c r="F12" s="58" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="G12" s="58" t="inlineStr">
+        <is>
+          <t>Swing</t>
+        </is>
+      </c>
+      <c r="H12" s="37" t="inlineStr">
+        <is>
+          <t>Foul</t>
+        </is>
+      </c>
       <c r="I12" s="61" t="inlineStr">
         <is>
           <t>Runners:</t>
@@ -1347,16 +1387,32 @@
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M12" s="54" t="inlineStr"/>
+      <c r="M12" s="54" t="inlineStr">
+        <is>
+          <t>14.57°</t>
+        </is>
+      </c>
       <c r="N12" s="93" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1" thickBot="1">
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="23" t="n"/>
       <c r="E13" s="23" t="n"/>
-      <c r="F13" s="58" t="n"/>
-      <c r="G13" s="58" t="n"/>
-      <c r="H13" s="37" t="n"/>
+      <c r="F13" s="58" t="inlineStr">
+        <is>
+          <t>SL</t>
+        </is>
+      </c>
+      <c r="G13" s="58" t="inlineStr">
+        <is>
+          <t>Swing</t>
+        </is>
+      </c>
+      <c r="H13" s="37" t="inlineStr">
+        <is>
+          <t>In Play</t>
+        </is>
+      </c>
       <c r="I13" s="62" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
@@ -1467,7 +1523,7 @@
       </c>
       <c r="J17" s="46" t="inlineStr">
         <is>
-          <t>SL,FB,CH</t>
+          <t>CH,FB,SL</t>
         </is>
       </c>
       <c r="K17" s="97" t="n"/>
@@ -1517,9 +1573,17 @@
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="3" t="n"/>
       <c r="E19" s="3" t="n"/>
-      <c r="F19" s="57" t="n"/>
-      <c r="G19" s="57" t="n"/>
-      <c r="H19" s="36" t="n"/>
+      <c r="F19" s="57" t="inlineStr"/>
+      <c r="G19" s="57" t="inlineStr">
+        <is>
+          <t>Take</t>
+        </is>
+      </c>
+      <c r="H19" s="36" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
       <c r="I19" s="60" t="inlineStr">
         <is>
           <t>Inning:</t>
@@ -1534,16 +1598,32 @@
         </is>
       </c>
       <c r="L19" s="84" t="n"/>
-      <c r="M19" s="52" t="inlineStr"/>
+      <c r="M19" s="52" t="inlineStr">
+        <is>
+          <t>61.48 MPH</t>
+        </is>
+      </c>
       <c r="N19" s="87" t="n"/>
     </row>
     <row r="20" ht="14.5" customHeight="1">
       <c r="C20" s="4" t="n"/>
       <c r="D20" s="23" t="n"/>
       <c r="E20" s="23" t="n"/>
-      <c r="F20" s="58" t="n"/>
-      <c r="G20" s="58" t="n"/>
-      <c r="H20" s="37" t="n"/>
+      <c r="F20" s="58" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="G20" s="58" t="inlineStr">
+        <is>
+          <t>Take</t>
+        </is>
+      </c>
+      <c r="H20" s="37" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
       <c r="I20" s="48" t="inlineStr">
         <is>
           <t>Outs:</t>
@@ -1559,9 +1639,21 @@
       <c r="C21" s="4" t="n"/>
       <c r="D21" s="23" t="n"/>
       <c r="E21" s="23" t="n"/>
-      <c r="F21" s="58" t="n"/>
-      <c r="G21" s="58" t="n"/>
-      <c r="H21" s="37" t="n"/>
+      <c r="F21" s="58" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="G21" s="58" t="inlineStr">
+        <is>
+          <t>Take</t>
+        </is>
+      </c>
+      <c r="H21" s="37" t="inlineStr">
+        <is>
+          <t>Ball</t>
+        </is>
+      </c>
       <c r="I21" s="61" t="inlineStr">
         <is>
           <t>Runners:</t>
@@ -1577,16 +1669,32 @@
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M21" s="54" t="inlineStr"/>
+      <c r="M21" s="54" t="inlineStr">
+        <is>
+          <t>14.14°</t>
+        </is>
+      </c>
       <c r="N21" s="93" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1" thickBot="1">
       <c r="C22" s="4" t="n"/>
       <c r="D22" s="23" t="n"/>
       <c r="E22" s="23" t="n"/>
-      <c r="F22" s="58" t="n"/>
-      <c r="G22" s="58" t="n"/>
-      <c r="H22" s="37" t="n"/>
+      <c r="F22" s="58" t="inlineStr">
+        <is>
+          <t>FB</t>
+        </is>
+      </c>
+      <c r="G22" s="58" t="inlineStr">
+        <is>
+          <t>Take</t>
+        </is>
+      </c>
+      <c r="H22" s="37" t="inlineStr">
+        <is>
+          <t>Strike</t>
+        </is>
+      </c>
       <c r="I22" s="62" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
@@ -1600,9 +1708,21 @@
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="23" t="n"/>
       <c r="E23" s="23" t="n"/>
-      <c r="F23" s="58" t="n"/>
-      <c r="G23" s="58" t="n"/>
-      <c r="H23" s="37" t="n"/>
+      <c r="F23" s="58" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="G23" s="58" t="inlineStr">
+        <is>
+          <t>Swing</t>
+        </is>
+      </c>
+      <c r="H23" s="37" t="inlineStr">
+        <is>
+          <t>In Play</t>
+        </is>
+      </c>
       <c r="I23" s="60" t="inlineStr">
         <is>
           <t>Name:</t>
@@ -1697,7 +1817,7 @@
       </c>
       <c r="J26" s="46" t="inlineStr">
         <is>
-          <t>SL,FB,CH</t>
+          <t>CH,FB,SL</t>
         </is>
       </c>
       <c r="K26" s="97" t="n"/>

</xml_diff>

<commit_message>
stopping to play mario party 8 with the boys
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -863,6 +863,61 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>8</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2057400" cy="4114800"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2057400" cy="4114800"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1523,7 +1578,7 @@
       </c>
       <c r="J17" s="46" t="inlineStr">
         <is>
-          <t>CH,FB,SL</t>
+          <t>FB,SL,CH</t>
         </is>
       </c>
       <c r="K17" s="97" t="n"/>
@@ -1817,7 +1872,7 @@
       </c>
       <c r="J26" s="46" t="inlineStr">
         <is>
-          <t>CH,FB,SL</t>
+          <t>FB,SL,CH</t>
         </is>
       </c>
       <c r="K26" s="97" t="n"/>
@@ -3632,5 +3687,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="53" min="2" max="13" man="1"/>
   </rowBreaks>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited hitter/pitcher code a bit, good progress
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -78,6 +78,14 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -608,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" textRotation="45"/>
@@ -685,181 +693,193 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1226,7 +1246,7 @@
   <dimension ref="C3:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1245,105 +1265,105 @@
   <sheetData>
     <row r="2" ht="15" customHeight="1" thickBot="1"/>
     <row r="3" ht="9.5" customHeight="1">
-      <c r="C3" s="49" t="inlineStr">
+      <c r="C3" s="57" t="inlineStr">
         <is>
           <t>Advincula, Jonah</t>
         </is>
       </c>
-      <c r="D3" s="85" t="n"/>
-      <c r="E3" s="86" t="n"/>
-      <c r="F3" s="64" t="inlineStr">
+      <c r="D3" s="89" t="n"/>
+      <c r="E3" s="90" t="n"/>
+      <c r="F3" s="49" t="inlineStr">
         <is>
           <t>RyLar Baseball</t>
         </is>
       </c>
-      <c r="G3" s="85" t="n"/>
-      <c r="H3" s="85" t="n"/>
-      <c r="I3" s="85" t="n"/>
-      <c r="J3" s="85" t="n"/>
-      <c r="K3" s="85" t="n"/>
-      <c r="L3" s="86" t="n"/>
-      <c r="M3" s="87" t="n"/>
-      <c r="N3" s="88" t="n"/>
+      <c r="G3" s="89" t="n"/>
+      <c r="H3" s="89" t="n"/>
+      <c r="I3" s="89" t="n"/>
+      <c r="J3" s="89" t="n"/>
+      <c r="K3" s="89" t="n"/>
+      <c r="L3" s="90" t="n"/>
+      <c r="M3" s="91" t="n"/>
+      <c r="N3" s="92" t="n"/>
     </row>
     <row r="4" ht="14.5" customHeight="1">
-      <c r="C4" s="89" t="n"/>
-      <c r="D4" s="90" t="n"/>
-      <c r="E4" s="91" t="n"/>
-      <c r="F4" s="92" t="n"/>
-      <c r="L4" s="93" t="n"/>
-      <c r="M4" s="92" t="n"/>
-      <c r="N4" s="94" t="n"/>
+      <c r="C4" s="93" t="n"/>
+      <c r="D4" s="94" t="n"/>
+      <c r="E4" s="95" t="n"/>
+      <c r="F4" s="96" t="n"/>
+      <c r="L4" s="97" t="n"/>
+      <c r="M4" s="96" t="n"/>
+      <c r="N4" s="98" t="n"/>
     </row>
     <row r="5" ht="7" customHeight="1">
-      <c r="C5" s="55" t="n">
+      <c r="C5" s="67" t="n">
         <v>44771</v>
       </c>
-      <c r="D5" s="95" t="n"/>
-      <c r="E5" s="96" t="n"/>
-      <c r="F5" s="89" t="n"/>
-      <c r="G5" s="90" t="n"/>
-      <c r="H5" s="90" t="n"/>
-      <c r="I5" s="90" t="n"/>
-      <c r="J5" s="90" t="n"/>
-      <c r="K5" s="90" t="n"/>
-      <c r="L5" s="91" t="n"/>
-      <c r="M5" s="92" t="n"/>
-      <c r="N5" s="94" t="n"/>
+      <c r="D5" s="99" t="n"/>
+      <c r="E5" s="100" t="n"/>
+      <c r="F5" s="93" t="n"/>
+      <c r="G5" s="94" t="n"/>
+      <c r="H5" s="94" t="n"/>
+      <c r="I5" s="94" t="n"/>
+      <c r="J5" s="94" t="n"/>
+      <c r="K5" s="94" t="n"/>
+      <c r="L5" s="95" t="n"/>
+      <c r="M5" s="96" t="n"/>
+      <c r="N5" s="98" t="n"/>
     </row>
     <row r="6" ht="14.5" customHeight="1">
-      <c r="C6" s="89" t="n"/>
-      <c r="D6" s="90" t="n"/>
-      <c r="E6" s="91" t="n"/>
-      <c r="F6" s="72" t="inlineStr">
+      <c r="C6" s="93" t="n"/>
+      <c r="D6" s="94" t="n"/>
+      <c r="E6" s="95" t="n"/>
+      <c r="F6" s="70" t="inlineStr">
         <is>
           <t>Postgame Hitting Report</t>
         </is>
       </c>
-      <c r="G6" s="95" t="n"/>
-      <c r="H6" s="95" t="n"/>
-      <c r="I6" s="95" t="n"/>
-      <c r="J6" s="95" t="n"/>
-      <c r="K6" s="95" t="n"/>
-      <c r="L6" s="96" t="n"/>
-      <c r="M6" s="92" t="n"/>
-      <c r="N6" s="94" t="n"/>
+      <c r="G6" s="99" t="n"/>
+      <c r="H6" s="99" t="n"/>
+      <c r="I6" s="99" t="n"/>
+      <c r="J6" s="99" t="n"/>
+      <c r="K6" s="99" t="n"/>
+      <c r="L6" s="100" t="n"/>
+      <c r="M6" s="96" t="n"/>
+      <c r="N6" s="98" t="n"/>
     </row>
     <row r="7" ht="14.5" customHeight="1">
-      <c r="C7" s="58" t="inlineStr">
+      <c r="C7" s="78" t="inlineStr">
         <is>
           <t>v Sweets</t>
         </is>
       </c>
-      <c r="D7" s="95" t="n"/>
-      <c r="E7" s="96" t="n"/>
-      <c r="F7" s="92" t="n"/>
-      <c r="L7" s="93" t="n"/>
-      <c r="M7" s="92" t="n"/>
-      <c r="N7" s="94" t="n"/>
+      <c r="D7" s="99" t="n"/>
+      <c r="E7" s="100" t="n"/>
+      <c r="F7" s="96" t="n"/>
+      <c r="L7" s="97" t="n"/>
+      <c r="M7" s="96" t="n"/>
+      <c r="N7" s="98" t="n"/>
     </row>
     <row r="8" ht="6.5" customHeight="1" thickBot="1">
-      <c r="C8" s="89" t="n"/>
-      <c r="D8" s="90" t="n"/>
-      <c r="E8" s="91" t="n"/>
-      <c r="F8" s="89" t="n"/>
-      <c r="G8" s="90" t="n"/>
-      <c r="H8" s="90" t="n"/>
-      <c r="I8" s="90" t="n"/>
-      <c r="J8" s="90" t="n"/>
-      <c r="K8" s="90" t="n"/>
-      <c r="L8" s="91" t="n"/>
-      <c r="M8" s="92" t="n"/>
-      <c r="N8" s="94" t="n"/>
+      <c r="C8" s="93" t="n"/>
+      <c r="D8" s="94" t="n"/>
+      <c r="E8" s="95" t="n"/>
+      <c r="F8" s="93" t="n"/>
+      <c r="G8" s="94" t="n"/>
+      <c r="H8" s="94" t="n"/>
+      <c r="I8" s="94" t="n"/>
+      <c r="J8" s="94" t="n"/>
+      <c r="K8" s="94" t="n"/>
+      <c r="L8" s="95" t="n"/>
+      <c r="M8" s="96" t="n"/>
+      <c r="N8" s="98" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1" thickBot="1">
-      <c r="C9" s="37" t="inlineStr">
+      <c r="C9" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D9" s="85" t="n"/>
-      <c r="E9" s="86" t="n"/>
+      <c r="D9" s="89" t="n"/>
+      <c r="E9" s="90" t="n"/>
       <c r="F9" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -1359,26 +1379,26 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I9" s="42" t="inlineStr">
+      <c r="I9" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J9" s="86" t="n"/>
-      <c r="K9" s="42" t="inlineStr">
+      <c r="J9" s="90" t="n"/>
+      <c r="K9" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L9" s="85" t="n"/>
-      <c r="M9" s="85" t="n"/>
-      <c r="N9" s="86" t="n"/>
+      <c r="L9" s="89" t="n"/>
+      <c r="M9" s="89" t="n"/>
+      <c r="N9" s="90" t="n"/>
     </row>
     <row r="10" ht="14.5" customHeight="1">
       <c r="C10" s="2" t="n"/>
       <c r="D10" s="3" t="n"/>
       <c r="E10" s="3" t="n"/>
-      <c r="F10" s="97" t="inlineStr">
+      <c r="F10" s="101" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
@@ -1388,37 +1408,37 @@
           <t>Take</t>
         </is>
       </c>
-      <c r="H10" s="10" t="inlineStr">
+      <c r="H10" s="85" t="inlineStr">
         <is>
           <t>Strike</t>
         </is>
       </c>
-      <c r="I10" s="32" t="inlineStr">
+      <c r="I10" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J10" s="83" t="n">
+      <c r="J10" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="K10" s="33" t="inlineStr">
+      <c r="K10" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L10" s="85" t="n"/>
-      <c r="M10" s="35" t="inlineStr">
+      <c r="L10" s="89" t="n"/>
+      <c r="M10" s="48" t="inlineStr">
         <is>
           <t>75.42 MPH</t>
         </is>
       </c>
-      <c r="N10" s="88" t="n"/>
+      <c r="N10" s="92" t="n"/>
     </row>
     <row r="11">
       <c r="C11" s="4" t="n"/>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
-      <c r="F11" s="98" t="inlineStr">
+      <c r="F11" s="102" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
@@ -1428,26 +1448,26 @@
           <t>Swing</t>
         </is>
       </c>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="H11" s="86" t="inlineStr">
         <is>
           <t>Foul</t>
         </is>
       </c>
-      <c r="I11" s="26" t="inlineStr">
+      <c r="I11" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J11" s="29" t="n">
+      <c r="J11" s="38" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="94" t="n"/>
+      <c r="N11" s="98" t="n"/>
     </row>
     <row r="12">
       <c r="C12" s="4" t="n"/>
       <c r="D12" s="1" t="n"/>
       <c r="E12" s="1" t="n"/>
-      <c r="F12" s="99" t="inlineStr">
+      <c r="F12" s="103" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
@@ -1457,38 +1477,38 @@
           <t>Swing</t>
         </is>
       </c>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="H12" s="86" t="inlineStr">
         <is>
           <t>Foul</t>
         </is>
       </c>
-      <c r="I12" s="26" t="inlineStr">
+      <c r="I12" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J12" s="29" t="inlineStr">
+      <c r="J12" s="38" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="K12" s="80" t="inlineStr">
+      <c r="K12" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M12" s="36" t="inlineStr">
+      <c r="M12" s="34" t="inlineStr">
         <is>
           <t>14.57°</t>
         </is>
       </c>
-      <c r="N12" s="94" t="n"/>
+      <c r="N12" s="98" t="n"/>
     </row>
     <row r="13">
       <c r="C13" s="4" t="n"/>
       <c r="D13" s="1" t="n"/>
       <c r="E13" s="1" t="n"/>
-      <c r="F13" s="99" t="inlineStr">
+      <c r="F13" s="103" t="inlineStr">
         <is>
           <t>SL</t>
         </is>
@@ -1498,22 +1518,22 @@
           <t>Swing</t>
         </is>
       </c>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="H13" s="86" t="inlineStr">
         <is>
           <t>In Play</t>
         </is>
       </c>
-      <c r="I13" s="26" t="inlineStr">
+      <c r="I13" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J13" s="29" t="inlineStr">
+      <c r="J13" s="38" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="N13" s="94" t="n"/>
+      <c r="N13" s="98" t="n"/>
     </row>
     <row r="14" ht="15" customHeight="1" thickBot="1">
       <c r="C14" s="4" t="n"/>
@@ -1521,28 +1541,28 @@
       <c r="E14" s="1" t="n"/>
       <c r="F14" s="22" t="n"/>
       <c r="G14" s="22" t="n"/>
-      <c r="H14" s="11" t="n"/>
-      <c r="I14" s="27" t="inlineStr">
+      <c r="H14" s="86" t="n"/>
+      <c r="I14" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J14" s="84" t="inlineStr">
+      <c r="J14" s="88" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="K14" s="80" t="inlineStr">
+      <c r="K14" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M14" s="36" t="inlineStr">
+      <c r="M14" s="34" t="inlineStr">
         <is>
           <t>Line Drive</t>
         </is>
       </c>
-      <c r="N14" s="94" t="n"/>
+      <c r="N14" s="98" t="n"/>
     </row>
     <row r="15" ht="15" customHeight="1" thickBot="1">
       <c r="C15" s="4" t="n"/>
@@ -1550,14 +1570,14 @@
       <c r="E15" s="1" t="n"/>
       <c r="F15" s="22" t="n"/>
       <c r="G15" s="22" t="n"/>
-      <c r="H15" s="11" t="n"/>
-      <c r="I15" s="40" t="inlineStr">
+      <c r="H15" s="86" t="n"/>
+      <c r="I15" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J15" s="100" t="n"/>
-      <c r="N15" s="94" t="n"/>
+      <c r="J15" s="104" t="n"/>
+      <c r="N15" s="98" t="n"/>
     </row>
     <row r="16">
       <c r="C16" s="4" t="n"/>
@@ -1565,8 +1585,8 @@
       <c r="E16" s="1" t="n"/>
       <c r="F16" s="22" t="n"/>
       <c r="G16" s="22" t="n"/>
-      <c r="H16" s="11" t="n"/>
-      <c r="I16" s="33" t="inlineStr">
+      <c r="H16" s="86" t="n"/>
+      <c r="I16" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
@@ -1576,17 +1596,17 @@
           <t>Plum</t>
         </is>
       </c>
-      <c r="K16" s="26" t="inlineStr">
+      <c r="K16" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M16" s="29" t="inlineStr">
+      <c r="M16" s="38" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="N16" s="94" t="n"/>
+      <c r="N16" s="98" t="n"/>
     </row>
     <row r="17">
       <c r="C17" s="4" t="n"/>
@@ -1594,19 +1614,19 @@
       <c r="E17" s="1" t="n"/>
       <c r="F17" s="22" t="n"/>
       <c r="G17" s="22" t="n"/>
-      <c r="H17" s="11" t="n"/>
-      <c r="I17" s="80" t="inlineStr">
+      <c r="H17" s="86" t="n"/>
+      <c r="I17" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J17" s="82" t="inlineStr">
+      <c r="J17" s="37" t="inlineStr">
         <is>
           <t>Right</t>
         </is>
       </c>
-      <c r="K17" s="92" t="n"/>
-      <c r="N17" s="94" t="n"/>
+      <c r="K17" s="96" t="n"/>
+      <c r="N17" s="98" t="n"/>
     </row>
     <row r="18">
       <c r="C18" s="4" t="n"/>
@@ -1614,28 +1634,24 @@
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="22" t="n"/>
       <c r="G18" s="22" t="n"/>
-      <c r="H18" s="11" t="n"/>
-      <c r="I18" s="80" t="inlineStr">
+      <c r="H18" s="86" t="n"/>
+      <c r="I18" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
-      <c r="J18" s="14" t="inlineStr">
-        <is>
-          <t>84-86 MPH</t>
-        </is>
-      </c>
-      <c r="K18" s="27" t="inlineStr">
+      <c r="J18" s="14" t="n"/>
+      <c r="K18" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M18" s="31" t="inlineStr">
+      <c r="M18" s="42" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="N18" s="94" t="n"/>
+      <c r="N18" s="98" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1" thickBot="1">
       <c r="C19" s="5" t="n"/>
@@ -1643,30 +1659,30 @@
       <c r="E19" s="6" t="n"/>
       <c r="F19" s="23" t="n"/>
       <c r="G19" s="23" t="n"/>
-      <c r="H19" s="25" t="n"/>
-      <c r="I19" s="28" t="inlineStr">
+      <c r="H19" s="87" t="n"/>
+      <c r="I19" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J19" s="17" t="inlineStr">
         <is>
-          <t>SL,CH,FB</t>
-        </is>
-      </c>
-      <c r="K19" s="101" t="n"/>
-      <c r="L19" s="102" t="n"/>
-      <c r="M19" s="102" t="n"/>
-      <c r="N19" s="84" t="n"/>
+          <t>CH,FB,SL</t>
+        </is>
+      </c>
+      <c r="K19" s="105" t="n"/>
+      <c r="L19" s="106" t="n"/>
+      <c r="M19" s="106" t="n"/>
+      <c r="N19" s="27" t="n"/>
     </row>
     <row r="20" ht="15" customHeight="1" thickBot="1">
-      <c r="C20" s="37" t="inlineStr">
+      <c r="C20" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D20" s="85" t="n"/>
-      <c r="E20" s="86" t="n"/>
+      <c r="D20" s="89" t="n"/>
+      <c r="E20" s="90" t="n"/>
       <c r="F20" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -1682,26 +1698,26 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I20" s="42" t="inlineStr">
+      <c r="I20" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J20" s="86" t="n"/>
-      <c r="K20" s="42" t="inlineStr">
+      <c r="J20" s="90" t="n"/>
+      <c r="K20" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L20" s="85" t="n"/>
-      <c r="M20" s="85" t="n"/>
-      <c r="N20" s="86" t="n"/>
+      <c r="L20" s="89" t="n"/>
+      <c r="M20" s="89" t="n"/>
+      <c r="N20" s="90" t="n"/>
     </row>
     <row r="21" ht="14.5" customHeight="1">
       <c r="C21" s="2" t="n"/>
       <c r="D21" s="3" t="n"/>
       <c r="E21" s="3" t="n"/>
-      <c r="F21" s="103" t="inlineStr"/>
+      <c r="F21" s="107" t="inlineStr"/>
       <c r="G21" s="21" t="inlineStr">
         <is>
           <t>Take</t>
@@ -1712,32 +1728,32 @@
           <t>Ball</t>
         </is>
       </c>
-      <c r="I21" s="32" t="inlineStr">
+      <c r="I21" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J21" s="83" t="n">
+      <c r="J21" s="26" t="n">
         <v>7</v>
       </c>
-      <c r="K21" s="33" t="inlineStr">
+      <c r="K21" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L21" s="85" t="n"/>
-      <c r="M21" s="35" t="inlineStr">
+      <c r="L21" s="89" t="n"/>
+      <c r="M21" s="48" t="inlineStr">
         <is>
           <t>61.48 MPH</t>
         </is>
       </c>
-      <c r="N21" s="88" t="n"/>
+      <c r="N21" s="92" t="n"/>
     </row>
     <row r="22">
       <c r="C22" s="4" t="n"/>
       <c r="D22" s="1" t="n"/>
       <c r="E22" s="1" t="n"/>
-      <c r="F22" s="104" t="inlineStr">
+      <c r="F22" s="108" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
@@ -1752,21 +1768,21 @@
           <t>Strike</t>
         </is>
       </c>
-      <c r="I22" s="26" t="inlineStr">
+      <c r="I22" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J22" s="29" t="n">
+      <c r="J22" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="N22" s="94" t="n"/>
+      <c r="N22" s="98" t="n"/>
     </row>
     <row r="23">
       <c r="C23" s="4" t="n"/>
       <c r="D23" s="1" t="n"/>
       <c r="E23" s="1" t="n"/>
-      <c r="F23" s="104" t="inlineStr">
+      <c r="F23" s="108" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
@@ -1781,33 +1797,33 @@
           <t>Ball</t>
         </is>
       </c>
-      <c r="I23" s="26" t="inlineStr">
+      <c r="I23" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J23" s="29" t="inlineStr">
+      <c r="J23" s="38" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="K23" s="80" t="inlineStr">
+      <c r="K23" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M23" s="36" t="inlineStr">
+      <c r="M23" s="34" t="inlineStr">
         <is>
           <t>14.14°</t>
         </is>
       </c>
-      <c r="N23" s="94" t="n"/>
+      <c r="N23" s="98" t="n"/>
     </row>
     <row r="24">
       <c r="C24" s="4" t="n"/>
       <c r="D24" s="1" t="n"/>
       <c r="E24" s="1" t="n"/>
-      <c r="F24" s="98" t="inlineStr">
+      <c r="F24" s="102" t="inlineStr">
         <is>
           <t>FB</t>
         </is>
@@ -1822,23 +1838,23 @@
           <t>Strike</t>
         </is>
       </c>
-      <c r="I24" s="26" t="inlineStr">
+      <c r="I24" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J24" s="29" t="inlineStr">
+      <c r="J24" s="38" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="N24" s="94" t="n"/>
+      <c r="N24" s="98" t="n"/>
     </row>
     <row r="25" ht="15" customHeight="1" thickBot="1">
       <c r="C25" s="4" t="n"/>
       <c r="D25" s="1" t="n"/>
       <c r="E25" s="1" t="n"/>
-      <c r="F25" s="104" t="inlineStr">
+      <c r="F25" s="108" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
@@ -1853,27 +1869,27 @@
           <t>In Play</t>
         </is>
       </c>
-      <c r="I25" s="27" t="inlineStr">
+      <c r="I25" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J25" s="84" t="inlineStr">
+      <c r="J25" s="27" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="K25" s="80" t="inlineStr">
+      <c r="K25" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M25" s="36" t="inlineStr">
+      <c r="M25" s="34" t="inlineStr">
         <is>
           <t>Ground Ball</t>
         </is>
       </c>
-      <c r="N25" s="94" t="n"/>
+      <c r="N25" s="98" t="n"/>
     </row>
     <row r="26" ht="15" customHeight="1" thickBot="1">
       <c r="C26" s="4" t="n"/>
@@ -1882,13 +1898,13 @@
       <c r="F26" s="22" t="n"/>
       <c r="G26" s="22" t="n"/>
       <c r="H26" s="11" t="n"/>
-      <c r="I26" s="40" t="inlineStr">
+      <c r="I26" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J26" s="100" t="n"/>
-      <c r="N26" s="94" t="n"/>
+      <c r="J26" s="104" t="n"/>
+      <c r="N26" s="98" t="n"/>
     </row>
     <row r="27">
       <c r="C27" s="4" t="n"/>
@@ -1897,7 +1913,7 @@
       <c r="F27" s="22" t="n"/>
       <c r="G27" s="22" t="n"/>
       <c r="H27" s="11" t="n"/>
-      <c r="I27" s="33" t="inlineStr">
+      <c r="I27" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
@@ -1907,17 +1923,17 @@
           <t>Thompson</t>
         </is>
       </c>
-      <c r="K27" s="26" t="inlineStr">
+      <c r="K27" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M27" s="29" t="inlineStr">
+      <c r="M27" s="38" t="inlineStr">
         <is>
           <t>Out</t>
         </is>
       </c>
-      <c r="N27" s="94" t="n"/>
+      <c r="N27" s="98" t="n"/>
     </row>
     <row r="28">
       <c r="C28" s="4" t="n"/>
@@ -1926,18 +1942,18 @@
       <c r="F28" s="22" t="n"/>
       <c r="G28" s="22" t="n"/>
       <c r="H28" s="11" t="n"/>
-      <c r="I28" s="80" t="inlineStr">
+      <c r="I28" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J28" s="82" t="inlineStr">
+      <c r="J28" s="37" t="inlineStr">
         <is>
           <t>Left</t>
         </is>
       </c>
-      <c r="K28" s="92" t="n"/>
-      <c r="N28" s="94" t="n"/>
+      <c r="K28" s="96" t="n"/>
+      <c r="N28" s="98" t="n"/>
     </row>
     <row r="29">
       <c r="C29" s="4" t="n"/>
@@ -1946,7 +1962,7 @@
       <c r="F29" s="22" t="n"/>
       <c r="G29" s="22" t="n"/>
       <c r="H29" s="11" t="n"/>
-      <c r="I29" s="80" t="inlineStr">
+      <c r="I29" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
@@ -1956,17 +1972,17 @@
           <t>84-84 MPH</t>
         </is>
       </c>
-      <c r="K29" s="27" t="inlineStr">
+      <c r="K29" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M29" s="31" t="inlineStr">
+      <c r="M29" s="42" t="inlineStr">
         <is>
           <t>Coming Soon</t>
         </is>
       </c>
-      <c r="N29" s="94" t="n"/>
+      <c r="N29" s="98" t="n"/>
     </row>
     <row r="30" ht="15" customHeight="1" thickBot="1">
       <c r="C30" s="5" t="n"/>
@@ -1975,29 +1991,29 @@
       <c r="F30" s="23" t="n"/>
       <c r="G30" s="23" t="n"/>
       <c r="H30" s="25" t="n"/>
-      <c r="I30" s="28" t="inlineStr">
+      <c r="I30" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J30" s="17" t="inlineStr">
         <is>
-          <t>SL,CH,FB</t>
-        </is>
-      </c>
-      <c r="K30" s="101" t="n"/>
-      <c r="L30" s="102" t="n"/>
-      <c r="M30" s="102" t="n"/>
-      <c r="N30" s="84" t="n"/>
+          <t>CH,FB,SL</t>
+        </is>
+      </c>
+      <c r="K30" s="105" t="n"/>
+      <c r="L30" s="106" t="n"/>
+      <c r="M30" s="106" t="n"/>
+      <c r="N30" s="27" t="n"/>
     </row>
     <row r="31" ht="15" customHeight="1" thickBot="1">
-      <c r="C31" s="37" t="inlineStr">
+      <c r="C31" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D31" s="85" t="n"/>
-      <c r="E31" s="86" t="n"/>
+      <c r="D31" s="89" t="n"/>
+      <c r="E31" s="90" t="n"/>
       <c r="F31" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -2013,20 +2029,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I31" s="42" t="inlineStr">
+      <c r="I31" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J31" s="86" t="n"/>
-      <c r="K31" s="42" t="inlineStr">
+      <c r="J31" s="90" t="n"/>
+      <c r="K31" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L31" s="85" t="n"/>
-      <c r="M31" s="85" t="n"/>
-      <c r="N31" s="86" t="n"/>
+      <c r="L31" s="89" t="n"/>
+      <c r="M31" s="89" t="n"/>
+      <c r="N31" s="90" t="n"/>
     </row>
     <row r="32" ht="14.5" customHeight="1">
       <c r="C32" s="2" t="n"/>
@@ -2035,20 +2051,20 @@
       <c r="F32" s="21" t="n"/>
       <c r="G32" s="21" t="n"/>
       <c r="H32" s="10" t="n"/>
-      <c r="I32" s="32" t="inlineStr">
+      <c r="I32" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J32" s="83" t="n"/>
-      <c r="K32" s="33" t="inlineStr">
+      <c r="J32" s="26" t="n"/>
+      <c r="K32" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L32" s="85" t="n"/>
-      <c r="M32" s="35" t="n"/>
-      <c r="N32" s="88" t="n"/>
+      <c r="L32" s="89" t="n"/>
+      <c r="M32" s="48" t="n"/>
+      <c r="N32" s="92" t="n"/>
     </row>
     <row r="33">
       <c r="C33" s="4" t="n"/>
@@ -2057,13 +2073,13 @@
       <c r="F33" s="22" t="n"/>
       <c r="G33" s="22" t="n"/>
       <c r="H33" s="11" t="n"/>
-      <c r="I33" s="26" t="inlineStr">
+      <c r="I33" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J33" s="29" t="n"/>
-      <c r="N33" s="94" t="n"/>
+      <c r="J33" s="38" t="n"/>
+      <c r="N33" s="98" t="n"/>
     </row>
     <row r="34">
       <c r="C34" s="4" t="n"/>
@@ -2072,19 +2088,19 @@
       <c r="F34" s="22" t="n"/>
       <c r="G34" s="22" t="n"/>
       <c r="H34" s="11" t="n"/>
-      <c r="I34" s="26" t="inlineStr">
+      <c r="I34" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J34" s="29" t="n"/>
-      <c r="K34" s="80" t="inlineStr">
+      <c r="J34" s="38" t="n"/>
+      <c r="K34" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M34" s="36" t="n"/>
-      <c r="N34" s="94" t="n"/>
+      <c r="M34" s="34" t="n"/>
+      <c r="N34" s="98" t="n"/>
     </row>
     <row r="35">
       <c r="C35" s="4" t="n"/>
@@ -2093,13 +2109,13 @@
       <c r="F35" s="22" t="n"/>
       <c r="G35" s="22" t="n"/>
       <c r="H35" s="11" t="n"/>
-      <c r="I35" s="26" t="inlineStr">
+      <c r="I35" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J35" s="29" t="n"/>
-      <c r="N35" s="94" t="n"/>
+      <c r="J35" s="38" t="n"/>
+      <c r="N35" s="98" t="n"/>
     </row>
     <row r="36" ht="15" customHeight="1" thickBot="1">
       <c r="C36" s="4" t="n"/>
@@ -2108,19 +2124,19 @@
       <c r="F36" s="22" t="n"/>
       <c r="G36" s="22" t="n"/>
       <c r="H36" s="11" t="n"/>
-      <c r="I36" s="27" t="inlineStr">
+      <c r="I36" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J36" s="84" t="n"/>
-      <c r="K36" s="80" t="inlineStr">
+      <c r="J36" s="27" t="n"/>
+      <c r="K36" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M36" s="36" t="n"/>
-      <c r="N36" s="94" t="n"/>
+      <c r="M36" s="34" t="n"/>
+      <c r="N36" s="98" t="n"/>
     </row>
     <row r="37" ht="15" customHeight="1" thickBot="1">
       <c r="C37" s="4" t="n"/>
@@ -2129,13 +2145,13 @@
       <c r="F37" s="22" t="n"/>
       <c r="G37" s="22" t="n"/>
       <c r="H37" s="11" t="n"/>
-      <c r="I37" s="40" t="inlineStr">
+      <c r="I37" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J37" s="100" t="n"/>
-      <c r="N37" s="94" t="n"/>
+      <c r="J37" s="104" t="n"/>
+      <c r="N37" s="98" t="n"/>
     </row>
     <row r="38">
       <c r="C38" s="4" t="n"/>
@@ -2144,19 +2160,19 @@
       <c r="F38" s="22" t="n"/>
       <c r="G38" s="22" t="n"/>
       <c r="H38" s="11" t="n"/>
-      <c r="I38" s="33" t="inlineStr">
+      <c r="I38" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J38" s="16" t="n"/>
-      <c r="K38" s="26" t="inlineStr">
+      <c r="K38" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M38" s="29" t="n"/>
-      <c r="N38" s="94" t="n"/>
+      <c r="M38" s="38" t="n"/>
+      <c r="N38" s="98" t="n"/>
     </row>
     <row r="39">
       <c r="C39" s="4" t="n"/>
@@ -2165,14 +2181,14 @@
       <c r="F39" s="22" t="n"/>
       <c r="G39" s="22" t="n"/>
       <c r="H39" s="11" t="n"/>
-      <c r="I39" s="80" t="inlineStr">
+      <c r="I39" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J39" s="82" t="n"/>
-      <c r="K39" s="92" t="n"/>
-      <c r="N39" s="94" t="n"/>
+      <c r="J39" s="37" t="n"/>
+      <c r="K39" s="96" t="n"/>
+      <c r="N39" s="98" t="n"/>
     </row>
     <row r="40">
       <c r="C40" s="4" t="n"/>
@@ -2181,19 +2197,19 @@
       <c r="F40" s="22" t="n"/>
       <c r="G40" s="22" t="n"/>
       <c r="H40" s="11" t="n"/>
-      <c r="I40" s="80" t="inlineStr">
+      <c r="I40" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J40" s="14" t="n"/>
-      <c r="K40" s="27" t="inlineStr">
+      <c r="K40" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M40" s="31" t="n"/>
-      <c r="N40" s="94" t="n"/>
+      <c r="M40" s="42" t="n"/>
+      <c r="N40" s="98" t="n"/>
     </row>
     <row r="41" ht="15" customHeight="1" thickBot="1">
       <c r="C41" s="5" t="n"/>
@@ -2202,25 +2218,25 @@
       <c r="F41" s="23" t="n"/>
       <c r="G41" s="23" t="n"/>
       <c r="H41" s="25" t="n"/>
-      <c r="I41" s="28" t="inlineStr">
+      <c r="I41" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J41" s="17" t="n"/>
-      <c r="K41" s="101" t="n"/>
-      <c r="L41" s="102" t="n"/>
-      <c r="M41" s="102" t="n"/>
-      <c r="N41" s="84" t="n"/>
+      <c r="K41" s="105" t="n"/>
+      <c r="L41" s="106" t="n"/>
+      <c r="M41" s="106" t="n"/>
+      <c r="N41" s="27" t="n"/>
     </row>
     <row r="42" ht="15" customHeight="1" thickBot="1">
-      <c r="C42" s="37" t="inlineStr">
+      <c r="C42" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D42" s="85" t="n"/>
-      <c r="E42" s="86" t="n"/>
+      <c r="D42" s="89" t="n"/>
+      <c r="E42" s="90" t="n"/>
       <c r="F42" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -2236,20 +2252,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I42" s="42" t="inlineStr">
+      <c r="I42" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J42" s="86" t="n"/>
-      <c r="K42" s="42" t="inlineStr">
+      <c r="J42" s="90" t="n"/>
+      <c r="K42" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L42" s="85" t="n"/>
-      <c r="M42" s="85" t="n"/>
-      <c r="N42" s="86" t="n"/>
+      <c r="L42" s="89" t="n"/>
+      <c r="M42" s="89" t="n"/>
+      <c r="N42" s="90" t="n"/>
     </row>
     <row r="43" ht="14.5" customHeight="1">
       <c r="C43" s="2" t="n"/>
@@ -2258,20 +2274,20 @@
       <c r="F43" s="21" t="n"/>
       <c r="G43" s="21" t="n"/>
       <c r="H43" s="10" t="n"/>
-      <c r="I43" s="32" t="inlineStr">
+      <c r="I43" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J43" s="83" t="n"/>
-      <c r="K43" s="33" t="inlineStr">
+      <c r="J43" s="26" t="n"/>
+      <c r="K43" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L43" s="85" t="n"/>
-      <c r="M43" s="35" t="n"/>
-      <c r="N43" s="88" t="n"/>
+      <c r="L43" s="89" t="n"/>
+      <c r="M43" s="48" t="n"/>
+      <c r="N43" s="92" t="n"/>
     </row>
     <row r="44">
       <c r="C44" s="4" t="n"/>
@@ -2280,13 +2296,13 @@
       <c r="F44" s="22" t="n"/>
       <c r="G44" s="22" t="n"/>
       <c r="H44" s="11" t="n"/>
-      <c r="I44" s="26" t="inlineStr">
+      <c r="I44" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J44" s="29" t="n"/>
-      <c r="N44" s="94" t="n"/>
+      <c r="J44" s="38" t="n"/>
+      <c r="N44" s="98" t="n"/>
     </row>
     <row r="45">
       <c r="C45" s="4" t="n"/>
@@ -2295,19 +2311,19 @@
       <c r="F45" s="22" t="n"/>
       <c r="G45" s="22" t="n"/>
       <c r="H45" s="11" t="n"/>
-      <c r="I45" s="26" t="inlineStr">
+      <c r="I45" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J45" s="29" t="n"/>
-      <c r="K45" s="80" t="inlineStr">
+      <c r="J45" s="38" t="n"/>
+      <c r="K45" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M45" s="36" t="n"/>
-      <c r="N45" s="94" t="n"/>
+      <c r="M45" s="34" t="n"/>
+      <c r="N45" s="98" t="n"/>
     </row>
     <row r="46">
       <c r="C46" s="4" t="n"/>
@@ -2316,13 +2332,13 @@
       <c r="F46" s="22" t="n"/>
       <c r="G46" s="22" t="n"/>
       <c r="H46" s="11" t="n"/>
-      <c r="I46" s="26" t="inlineStr">
+      <c r="I46" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J46" s="29" t="n"/>
-      <c r="N46" s="94" t="n"/>
+      <c r="J46" s="38" t="n"/>
+      <c r="N46" s="98" t="n"/>
     </row>
     <row r="47" ht="15" customHeight="1" thickBot="1">
       <c r="C47" s="4" t="n"/>
@@ -2331,19 +2347,19 @@
       <c r="F47" s="22" t="n"/>
       <c r="G47" s="22" t="n"/>
       <c r="H47" s="11" t="n"/>
-      <c r="I47" s="27" t="inlineStr">
+      <c r="I47" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J47" s="84" t="n"/>
-      <c r="K47" s="80" t="inlineStr">
+      <c r="J47" s="27" t="n"/>
+      <c r="K47" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M47" s="36" t="n"/>
-      <c r="N47" s="94" t="n"/>
+      <c r="M47" s="34" t="n"/>
+      <c r="N47" s="98" t="n"/>
     </row>
     <row r="48" ht="15" customHeight="1" thickBot="1">
       <c r="C48" s="4" t="n"/>
@@ -2352,13 +2368,13 @@
       <c r="F48" s="22" t="n"/>
       <c r="G48" s="22" t="n"/>
       <c r="H48" s="11" t="n"/>
-      <c r="I48" s="40" t="inlineStr">
+      <c r="I48" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J48" s="100" t="n"/>
-      <c r="N48" s="94" t="n"/>
+      <c r="J48" s="104" t="n"/>
+      <c r="N48" s="98" t="n"/>
     </row>
     <row r="49">
       <c r="C49" s="4" t="n"/>
@@ -2367,19 +2383,19 @@
       <c r="F49" s="22" t="n"/>
       <c r="G49" s="22" t="n"/>
       <c r="H49" s="11" t="n"/>
-      <c r="I49" s="33" t="inlineStr">
+      <c r="I49" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J49" s="16" t="n"/>
-      <c r="K49" s="26" t="inlineStr">
+      <c r="K49" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M49" s="29" t="n"/>
-      <c r="N49" s="94" t="n"/>
+      <c r="M49" s="38" t="n"/>
+      <c r="N49" s="98" t="n"/>
     </row>
     <row r="50">
       <c r="C50" s="4" t="n"/>
@@ -2388,14 +2404,14 @@
       <c r="F50" s="22" t="n"/>
       <c r="G50" s="22" t="n"/>
       <c r="H50" s="11" t="n"/>
-      <c r="I50" s="80" t="inlineStr">
+      <c r="I50" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J50" s="82" t="n"/>
-      <c r="K50" s="92" t="n"/>
-      <c r="N50" s="94" t="n"/>
+      <c r="J50" s="37" t="n"/>
+      <c r="K50" s="96" t="n"/>
+      <c r="N50" s="98" t="n"/>
     </row>
     <row r="51">
       <c r="C51" s="4" t="n"/>
@@ -2404,19 +2420,19 @@
       <c r="F51" s="22" t="n"/>
       <c r="G51" s="22" t="n"/>
       <c r="H51" s="11" t="n"/>
-      <c r="I51" s="80" t="inlineStr">
+      <c r="I51" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J51" s="14" t="n"/>
-      <c r="K51" s="27" t="inlineStr">
+      <c r="K51" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M51" s="31" t="n"/>
-      <c r="N51" s="94" t="n"/>
+      <c r="M51" s="42" t="n"/>
+      <c r="N51" s="98" t="n"/>
     </row>
     <row r="52" ht="15" customHeight="1" thickBot="1">
       <c r="C52" s="5" t="n"/>
@@ -2425,117 +2441,117 @@
       <c r="F52" s="23" t="n"/>
       <c r="G52" s="23" t="n"/>
       <c r="H52" s="25" t="n"/>
-      <c r="I52" s="28" t="inlineStr">
+      <c r="I52" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J52" s="17" t="n"/>
-      <c r="K52" s="101" t="n"/>
-      <c r="L52" s="102" t="n"/>
-      <c r="M52" s="102" t="n"/>
-      <c r="N52" s="84" t="n"/>
+      <c r="K52" s="105" t="n"/>
+      <c r="L52" s="106" t="n"/>
+      <c r="M52" s="106" t="n"/>
+      <c r="N52" s="27" t="n"/>
     </row>
     <row r="53" ht="9.5" customHeight="1">
-      <c r="C53" s="49" t="inlineStr">
+      <c r="C53" s="57" t="inlineStr">
         <is>
           <t>Advincula, Jonah</t>
         </is>
       </c>
-      <c r="D53" s="85" t="n"/>
-      <c r="E53" s="86" t="n"/>
-      <c r="F53" s="64" t="inlineStr">
+      <c r="D53" s="89" t="n"/>
+      <c r="E53" s="90" t="n"/>
+      <c r="F53" s="49" t="inlineStr">
         <is>
           <t>RyLar Baseball</t>
         </is>
       </c>
-      <c r="G53" s="85" t="n"/>
-      <c r="H53" s="85" t="n"/>
-      <c r="I53" s="85" t="n"/>
-      <c r="J53" s="85" t="n"/>
-      <c r="K53" s="85" t="n"/>
-      <c r="L53" s="86" t="n"/>
-      <c r="M53" s="87" t="n"/>
-      <c r="N53" s="88" t="n"/>
+      <c r="G53" s="89" t="n"/>
+      <c r="H53" s="89" t="n"/>
+      <c r="I53" s="89" t="n"/>
+      <c r="J53" s="89" t="n"/>
+      <c r="K53" s="89" t="n"/>
+      <c r="L53" s="90" t="n"/>
+      <c r="M53" s="91" t="n"/>
+      <c r="N53" s="92" t="n"/>
     </row>
     <row r="54" ht="14.5" customHeight="1">
-      <c r="C54" s="89" t="n"/>
-      <c r="D54" s="90" t="n"/>
-      <c r="E54" s="91" t="n"/>
-      <c r="F54" s="92" t="n"/>
-      <c r="L54" s="93" t="n"/>
-      <c r="M54" s="92" t="n"/>
-      <c r="N54" s="94" t="n"/>
+      <c r="C54" s="93" t="n"/>
+      <c r="D54" s="94" t="n"/>
+      <c r="E54" s="95" t="n"/>
+      <c r="F54" s="96" t="n"/>
+      <c r="L54" s="97" t="n"/>
+      <c r="M54" s="96" t="n"/>
+      <c r="N54" s="98" t="n"/>
     </row>
     <row r="55" ht="7" customHeight="1">
-      <c r="C55" s="55" t="n">
+      <c r="C55" s="67" t="n">
         <v>44771</v>
       </c>
-      <c r="D55" s="95" t="n"/>
-      <c r="E55" s="96" t="n"/>
-      <c r="F55" s="89" t="n"/>
-      <c r="G55" s="90" t="n"/>
-      <c r="H55" s="90" t="n"/>
-      <c r="I55" s="90" t="n"/>
-      <c r="J55" s="90" t="n"/>
-      <c r="K55" s="90" t="n"/>
-      <c r="L55" s="91" t="n"/>
-      <c r="M55" s="92" t="n"/>
-      <c r="N55" s="94" t="n"/>
+      <c r="D55" s="99" t="n"/>
+      <c r="E55" s="100" t="n"/>
+      <c r="F55" s="93" t="n"/>
+      <c r="G55" s="94" t="n"/>
+      <c r="H55" s="94" t="n"/>
+      <c r="I55" s="94" t="n"/>
+      <c r="J55" s="94" t="n"/>
+      <c r="K55" s="94" t="n"/>
+      <c r="L55" s="95" t="n"/>
+      <c r="M55" s="96" t="n"/>
+      <c r="N55" s="98" t="n"/>
     </row>
     <row r="56" ht="14.5" customHeight="1">
-      <c r="C56" s="89" t="n"/>
-      <c r="D56" s="90" t="n"/>
-      <c r="E56" s="91" t="n"/>
-      <c r="F56" s="72" t="inlineStr">
+      <c r="C56" s="93" t="n"/>
+      <c r="D56" s="94" t="n"/>
+      <c r="E56" s="95" t="n"/>
+      <c r="F56" s="70" t="inlineStr">
         <is>
           <t>Postgame Hitting Report</t>
         </is>
       </c>
-      <c r="G56" s="95" t="n"/>
-      <c r="H56" s="95" t="n"/>
-      <c r="I56" s="95" t="n"/>
-      <c r="J56" s="95" t="n"/>
-      <c r="K56" s="95" t="n"/>
-      <c r="L56" s="96" t="n"/>
-      <c r="M56" s="92" t="n"/>
-      <c r="N56" s="94" t="n"/>
+      <c r="G56" s="99" t="n"/>
+      <c r="H56" s="99" t="n"/>
+      <c r="I56" s="99" t="n"/>
+      <c r="J56" s="99" t="n"/>
+      <c r="K56" s="99" t="n"/>
+      <c r="L56" s="100" t="n"/>
+      <c r="M56" s="96" t="n"/>
+      <c r="N56" s="98" t="n"/>
     </row>
     <row r="57" ht="14.5" customHeight="1">
-      <c r="C57" s="58" t="inlineStr">
+      <c r="C57" s="78" t="inlineStr">
         <is>
           <t>v Sweets</t>
         </is>
       </c>
-      <c r="D57" s="95" t="n"/>
-      <c r="E57" s="96" t="n"/>
-      <c r="F57" s="92" t="n"/>
-      <c r="L57" s="93" t="n"/>
-      <c r="M57" s="92" t="n"/>
-      <c r="N57" s="94" t="n"/>
+      <c r="D57" s="99" t="n"/>
+      <c r="E57" s="100" t="n"/>
+      <c r="F57" s="96" t="n"/>
+      <c r="L57" s="97" t="n"/>
+      <c r="M57" s="96" t="n"/>
+      <c r="N57" s="98" t="n"/>
     </row>
     <row r="58" ht="6.5" customHeight="1" thickBot="1">
-      <c r="C58" s="89" t="n"/>
-      <c r="D58" s="90" t="n"/>
-      <c r="E58" s="91" t="n"/>
-      <c r="F58" s="89" t="n"/>
-      <c r="G58" s="90" t="n"/>
-      <c r="H58" s="90" t="n"/>
-      <c r="I58" s="90" t="n"/>
-      <c r="J58" s="90" t="n"/>
-      <c r="K58" s="90" t="n"/>
-      <c r="L58" s="91" t="n"/>
-      <c r="M58" s="92" t="n"/>
-      <c r="N58" s="94" t="n"/>
+      <c r="C58" s="93" t="n"/>
+      <c r="D58" s="94" t="n"/>
+      <c r="E58" s="95" t="n"/>
+      <c r="F58" s="93" t="n"/>
+      <c r="G58" s="94" t="n"/>
+      <c r="H58" s="94" t="n"/>
+      <c r="I58" s="94" t="n"/>
+      <c r="J58" s="94" t="n"/>
+      <c r="K58" s="94" t="n"/>
+      <c r="L58" s="95" t="n"/>
+      <c r="M58" s="96" t="n"/>
+      <c r="N58" s="98" t="n"/>
     </row>
     <row r="59" ht="15" customHeight="1" thickBot="1">
-      <c r="C59" s="37" t="inlineStr">
+      <c r="C59" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D59" s="85" t="n"/>
-      <c r="E59" s="86" t="n"/>
+      <c r="D59" s="89" t="n"/>
+      <c r="E59" s="90" t="n"/>
       <c r="F59" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -2551,20 +2567,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I59" s="42" t="inlineStr">
+      <c r="I59" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J59" s="86" t="n"/>
-      <c r="K59" s="42" t="inlineStr">
+      <c r="J59" s="90" t="n"/>
+      <c r="K59" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L59" s="85" t="n"/>
-      <c r="M59" s="85" t="n"/>
-      <c r="N59" s="86" t="n"/>
+      <c r="L59" s="89" t="n"/>
+      <c r="M59" s="89" t="n"/>
+      <c r="N59" s="90" t="n"/>
     </row>
     <row r="60" ht="14.5" customHeight="1">
       <c r="C60" s="2" t="n"/>
@@ -2573,20 +2589,20 @@
       <c r="F60" s="21" t="n"/>
       <c r="G60" s="21" t="n"/>
       <c r="H60" s="10" t="n"/>
-      <c r="I60" s="32" t="inlineStr">
+      <c r="I60" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J60" s="83" t="n"/>
-      <c r="K60" s="33" t="inlineStr">
+      <c r="J60" s="26" t="n"/>
+      <c r="K60" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L60" s="85" t="n"/>
-      <c r="M60" s="35" t="n"/>
-      <c r="N60" s="88" t="n"/>
+      <c r="L60" s="89" t="n"/>
+      <c r="M60" s="48" t="n"/>
+      <c r="N60" s="92" t="n"/>
     </row>
     <row r="61">
       <c r="C61" s="4" t="n"/>
@@ -2595,13 +2611,13 @@
       <c r="F61" s="22" t="n"/>
       <c r="G61" s="22" t="n"/>
       <c r="H61" s="11" t="n"/>
-      <c r="I61" s="26" t="inlineStr">
+      <c r="I61" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J61" s="29" t="n"/>
-      <c r="N61" s="94" t="n"/>
+      <c r="J61" s="38" t="n"/>
+      <c r="N61" s="98" t="n"/>
     </row>
     <row r="62">
       <c r="C62" s="4" t="n"/>
@@ -2610,19 +2626,19 @@
       <c r="F62" s="22" t="n"/>
       <c r="G62" s="22" t="n"/>
       <c r="H62" s="11" t="n"/>
-      <c r="I62" s="26" t="inlineStr">
+      <c r="I62" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J62" s="29" t="n"/>
-      <c r="K62" s="80" t="inlineStr">
+      <c r="J62" s="38" t="n"/>
+      <c r="K62" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M62" s="36" t="n"/>
-      <c r="N62" s="94" t="n"/>
+      <c r="M62" s="34" t="n"/>
+      <c r="N62" s="98" t="n"/>
     </row>
     <row r="63">
       <c r="C63" s="4" t="n"/>
@@ -2631,13 +2647,13 @@
       <c r="F63" s="22" t="n"/>
       <c r="G63" s="22" t="n"/>
       <c r="H63" s="11" t="n"/>
-      <c r="I63" s="26" t="inlineStr">
+      <c r="I63" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J63" s="29" t="n"/>
-      <c r="N63" s="94" t="n"/>
+      <c r="J63" s="38" t="n"/>
+      <c r="N63" s="98" t="n"/>
     </row>
     <row r="64" ht="15" customHeight="1" thickBot="1">
       <c r="C64" s="4" t="n"/>
@@ -2646,19 +2662,19 @@
       <c r="F64" s="22" t="n"/>
       <c r="G64" s="22" t="n"/>
       <c r="H64" s="11" t="n"/>
-      <c r="I64" s="27" t="inlineStr">
+      <c r="I64" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J64" s="84" t="n"/>
-      <c r="K64" s="80" t="inlineStr">
+      <c r="J64" s="27" t="n"/>
+      <c r="K64" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M64" s="36" t="n"/>
-      <c r="N64" s="94" t="n"/>
+      <c r="M64" s="34" t="n"/>
+      <c r="N64" s="98" t="n"/>
     </row>
     <row r="65" ht="15" customHeight="1" thickBot="1">
       <c r="C65" s="4" t="n"/>
@@ -2667,13 +2683,13 @@
       <c r="F65" s="22" t="n"/>
       <c r="G65" s="22" t="n"/>
       <c r="H65" s="11" t="n"/>
-      <c r="I65" s="40" t="inlineStr">
+      <c r="I65" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J65" s="100" t="n"/>
-      <c r="N65" s="94" t="n"/>
+      <c r="J65" s="104" t="n"/>
+      <c r="N65" s="98" t="n"/>
     </row>
     <row r="66">
       <c r="C66" s="4" t="n"/>
@@ -2682,19 +2698,19 @@
       <c r="F66" s="22" t="n"/>
       <c r="G66" s="22" t="n"/>
       <c r="H66" s="11" t="n"/>
-      <c r="I66" s="33" t="inlineStr">
+      <c r="I66" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J66" s="16" t="n"/>
-      <c r="K66" s="26" t="inlineStr">
+      <c r="K66" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M66" s="29" t="n"/>
-      <c r="N66" s="94" t="n"/>
+      <c r="M66" s="38" t="n"/>
+      <c r="N66" s="98" t="n"/>
     </row>
     <row r="67">
       <c r="C67" s="4" t="n"/>
@@ -2703,14 +2719,14 @@
       <c r="F67" s="22" t="n"/>
       <c r="G67" s="22" t="n"/>
       <c r="H67" s="11" t="n"/>
-      <c r="I67" s="80" t="inlineStr">
+      <c r="I67" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J67" s="82" t="n"/>
-      <c r="K67" s="92" t="n"/>
-      <c r="N67" s="94" t="n"/>
+      <c r="J67" s="37" t="n"/>
+      <c r="K67" s="96" t="n"/>
+      <c r="N67" s="98" t="n"/>
     </row>
     <row r="68">
       <c r="C68" s="4" t="n"/>
@@ -2719,19 +2735,19 @@
       <c r="F68" s="22" t="n"/>
       <c r="G68" s="22" t="n"/>
       <c r="H68" s="11" t="n"/>
-      <c r="I68" s="80" t="inlineStr">
+      <c r="I68" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J68" s="14" t="n"/>
-      <c r="K68" s="27" t="inlineStr">
+      <c r="K68" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M68" s="31" t="n"/>
-      <c r="N68" s="94" t="n"/>
+      <c r="M68" s="42" t="n"/>
+      <c r="N68" s="98" t="n"/>
     </row>
     <row r="69" ht="15" customHeight="1" thickBot="1">
       <c r="C69" s="5" t="n"/>
@@ -2740,25 +2756,25 @@
       <c r="F69" s="23" t="n"/>
       <c r="G69" s="23" t="n"/>
       <c r="H69" s="25" t="n"/>
-      <c r="I69" s="28" t="inlineStr">
+      <c r="I69" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J69" s="17" t="n"/>
-      <c r="K69" s="101" t="n"/>
-      <c r="L69" s="102" t="n"/>
-      <c r="M69" s="102" t="n"/>
-      <c r="N69" s="84" t="n"/>
+      <c r="K69" s="105" t="n"/>
+      <c r="L69" s="106" t="n"/>
+      <c r="M69" s="106" t="n"/>
+      <c r="N69" s="27" t="n"/>
     </row>
     <row r="70" ht="15" customHeight="1" thickBot="1">
-      <c r="C70" s="37" t="inlineStr">
+      <c r="C70" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D70" s="85" t="n"/>
-      <c r="E70" s="86" t="n"/>
+      <c r="D70" s="89" t="n"/>
+      <c r="E70" s="90" t="n"/>
       <c r="F70" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -2774,20 +2790,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I70" s="42" t="inlineStr">
+      <c r="I70" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J70" s="86" t="n"/>
-      <c r="K70" s="42" t="inlineStr">
+      <c r="J70" s="90" t="n"/>
+      <c r="K70" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L70" s="85" t="n"/>
-      <c r="M70" s="85" t="n"/>
-      <c r="N70" s="86" t="n"/>
+      <c r="L70" s="89" t="n"/>
+      <c r="M70" s="89" t="n"/>
+      <c r="N70" s="90" t="n"/>
     </row>
     <row r="71" ht="14.5" customHeight="1">
       <c r="C71" s="2" t="n"/>
@@ -2796,20 +2812,20 @@
       <c r="F71" s="21" t="n"/>
       <c r="G71" s="21" t="n"/>
       <c r="H71" s="10" t="n"/>
-      <c r="I71" s="32" t="inlineStr">
+      <c r="I71" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J71" s="83" t="n"/>
-      <c r="K71" s="33" t="inlineStr">
+      <c r="J71" s="26" t="n"/>
+      <c r="K71" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L71" s="85" t="n"/>
-      <c r="M71" s="35" t="n"/>
-      <c r="N71" s="88" t="n"/>
+      <c r="L71" s="89" t="n"/>
+      <c r="M71" s="48" t="n"/>
+      <c r="N71" s="92" t="n"/>
     </row>
     <row r="72">
       <c r="C72" s="4" t="n"/>
@@ -2818,13 +2834,13 @@
       <c r="F72" s="22" t="n"/>
       <c r="G72" s="22" t="n"/>
       <c r="H72" s="11" t="n"/>
-      <c r="I72" s="26" t="inlineStr">
+      <c r="I72" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J72" s="29" t="n"/>
-      <c r="N72" s="94" t="n"/>
+      <c r="J72" s="38" t="n"/>
+      <c r="N72" s="98" t="n"/>
     </row>
     <row r="73">
       <c r="C73" s="4" t="n"/>
@@ -2833,19 +2849,19 @@
       <c r="F73" s="22" t="n"/>
       <c r="G73" s="22" t="n"/>
       <c r="H73" s="11" t="n"/>
-      <c r="I73" s="26" t="inlineStr">
+      <c r="I73" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J73" s="29" t="n"/>
-      <c r="K73" s="80" t="inlineStr">
+      <c r="J73" s="38" t="n"/>
+      <c r="K73" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M73" s="36" t="n"/>
-      <c r="N73" s="94" t="n"/>
+      <c r="M73" s="34" t="n"/>
+      <c r="N73" s="98" t="n"/>
     </row>
     <row r="74">
       <c r="C74" s="4" t="n"/>
@@ -2854,13 +2870,13 @@
       <c r="F74" s="22" t="n"/>
       <c r="G74" s="22" t="n"/>
       <c r="H74" s="11" t="n"/>
-      <c r="I74" s="26" t="inlineStr">
+      <c r="I74" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J74" s="29" t="n"/>
-      <c r="N74" s="94" t="n"/>
+      <c r="J74" s="38" t="n"/>
+      <c r="N74" s="98" t="n"/>
     </row>
     <row r="75" ht="15" customHeight="1" thickBot="1">
       <c r="C75" s="4" t="n"/>
@@ -2869,19 +2885,19 @@
       <c r="F75" s="22" t="n"/>
       <c r="G75" s="22" t="n"/>
       <c r="H75" s="11" t="n"/>
-      <c r="I75" s="27" t="inlineStr">
+      <c r="I75" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J75" s="84" t="n"/>
-      <c r="K75" s="80" t="inlineStr">
+      <c r="J75" s="27" t="n"/>
+      <c r="K75" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M75" s="36" t="n"/>
-      <c r="N75" s="94" t="n"/>
+      <c r="M75" s="34" t="n"/>
+      <c r="N75" s="98" t="n"/>
     </row>
     <row r="76" ht="15" customHeight="1" thickBot="1">
       <c r="C76" s="4" t="n"/>
@@ -2890,13 +2906,13 @@
       <c r="F76" s="22" t="n"/>
       <c r="G76" s="22" t="n"/>
       <c r="H76" s="11" t="n"/>
-      <c r="I76" s="40" t="inlineStr">
+      <c r="I76" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J76" s="100" t="n"/>
-      <c r="N76" s="94" t="n"/>
+      <c r="J76" s="104" t="n"/>
+      <c r="N76" s="98" t="n"/>
     </row>
     <row r="77">
       <c r="C77" s="4" t="n"/>
@@ -2905,19 +2921,19 @@
       <c r="F77" s="22" t="n"/>
       <c r="G77" s="22" t="n"/>
       <c r="H77" s="11" t="n"/>
-      <c r="I77" s="33" t="inlineStr">
+      <c r="I77" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J77" s="16" t="n"/>
-      <c r="K77" s="26" t="inlineStr">
+      <c r="K77" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M77" s="29" t="n"/>
-      <c r="N77" s="94" t="n"/>
+      <c r="M77" s="38" t="n"/>
+      <c r="N77" s="98" t="n"/>
     </row>
     <row r="78">
       <c r="C78" s="4" t="n"/>
@@ -2926,14 +2942,14 @@
       <c r="F78" s="22" t="n"/>
       <c r="G78" s="22" t="n"/>
       <c r="H78" s="11" t="n"/>
-      <c r="I78" s="80" t="inlineStr">
+      <c r="I78" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J78" s="82" t="n"/>
-      <c r="K78" s="92" t="n"/>
-      <c r="N78" s="94" t="n"/>
+      <c r="J78" s="37" t="n"/>
+      <c r="K78" s="96" t="n"/>
+      <c r="N78" s="98" t="n"/>
     </row>
     <row r="79">
       <c r="C79" s="4" t="n"/>
@@ -2942,19 +2958,19 @@
       <c r="F79" s="22" t="n"/>
       <c r="G79" s="22" t="n"/>
       <c r="H79" s="11" t="n"/>
-      <c r="I79" s="80" t="inlineStr">
+      <c r="I79" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J79" s="14" t="n"/>
-      <c r="K79" s="27" t="inlineStr">
+      <c r="K79" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M79" s="31" t="n"/>
-      <c r="N79" s="94" t="n"/>
+      <c r="M79" s="42" t="n"/>
+      <c r="N79" s="98" t="n"/>
     </row>
     <row r="80" ht="15" customHeight="1" thickBot="1">
       <c r="C80" s="5" t="n"/>
@@ -2963,25 +2979,25 @@
       <c r="F80" s="23" t="n"/>
       <c r="G80" s="23" t="n"/>
       <c r="H80" s="25" t="n"/>
-      <c r="I80" s="28" t="inlineStr">
+      <c r="I80" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J80" s="17" t="n"/>
-      <c r="K80" s="101" t="n"/>
-      <c r="L80" s="102" t="n"/>
-      <c r="M80" s="102" t="n"/>
-      <c r="N80" s="84" t="n"/>
+      <c r="K80" s="105" t="n"/>
+      <c r="L80" s="106" t="n"/>
+      <c r="M80" s="106" t="n"/>
+      <c r="N80" s="27" t="n"/>
     </row>
     <row r="81" ht="15" customHeight="1" thickBot="1">
-      <c r="C81" s="37" t="inlineStr">
+      <c r="C81" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D81" s="85" t="n"/>
-      <c r="E81" s="86" t="n"/>
+      <c r="D81" s="89" t="n"/>
+      <c r="E81" s="90" t="n"/>
       <c r="F81" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -2997,20 +3013,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I81" s="42" t="inlineStr">
+      <c r="I81" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J81" s="86" t="n"/>
-      <c r="K81" s="42" t="inlineStr">
+      <c r="J81" s="90" t="n"/>
+      <c r="K81" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L81" s="85" t="n"/>
-      <c r="M81" s="85" t="n"/>
-      <c r="N81" s="86" t="n"/>
+      <c r="L81" s="89" t="n"/>
+      <c r="M81" s="89" t="n"/>
+      <c r="N81" s="90" t="n"/>
     </row>
     <row r="82" ht="14.5" customHeight="1">
       <c r="C82" s="2" t="n"/>
@@ -3019,20 +3035,20 @@
       <c r="F82" s="21" t="n"/>
       <c r="G82" s="21" t="n"/>
       <c r="H82" s="10" t="n"/>
-      <c r="I82" s="32" t="inlineStr">
+      <c r="I82" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J82" s="83" t="n"/>
-      <c r="K82" s="33" t="inlineStr">
+      <c r="J82" s="26" t="n"/>
+      <c r="K82" s="46" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L82" s="85" t="n"/>
-      <c r="M82" s="35" t="n"/>
-      <c r="N82" s="88" t="n"/>
+      <c r="L82" s="89" t="n"/>
+      <c r="M82" s="48" t="n"/>
+      <c r="N82" s="92" t="n"/>
     </row>
     <row r="83">
       <c r="C83" s="4" t="n"/>
@@ -3041,13 +3057,13 @@
       <c r="F83" s="22" t="n"/>
       <c r="G83" s="22" t="n"/>
       <c r="H83" s="11" t="n"/>
-      <c r="I83" s="26" t="inlineStr">
+      <c r="I83" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J83" s="29" t="n"/>
-      <c r="N83" s="94" t="n"/>
+      <c r="J83" s="38" t="n"/>
+      <c r="N83" s="98" t="n"/>
     </row>
     <row r="84">
       <c r="C84" s="4" t="n"/>
@@ -3056,19 +3072,19 @@
       <c r="F84" s="22" t="n"/>
       <c r="G84" s="22" t="n"/>
       <c r="H84" s="11" t="n"/>
-      <c r="I84" s="26" t="inlineStr">
+      <c r="I84" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J84" s="29" t="n"/>
-      <c r="K84" s="80" t="inlineStr">
+      <c r="J84" s="38" t="n"/>
+      <c r="K84" s="32" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M84" s="36" t="n"/>
-      <c r="N84" s="94" t="n"/>
+      <c r="M84" s="34" t="n"/>
+      <c r="N84" s="98" t="n"/>
     </row>
     <row r="85">
       <c r="C85" s="4" t="n"/>
@@ -3077,13 +3093,13 @@
       <c r="F85" s="22" t="n"/>
       <c r="G85" s="22" t="n"/>
       <c r="H85" s="11" t="n"/>
-      <c r="I85" s="26" t="inlineStr">
+      <c r="I85" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J85" s="29" t="n"/>
-      <c r="N85" s="94" t="n"/>
+      <c r="J85" s="38" t="n"/>
+      <c r="N85" s="98" t="n"/>
     </row>
     <row r="86" ht="15" customHeight="1" thickBot="1">
       <c r="C86" s="4" t="n"/>
@@ -3092,19 +3108,19 @@
       <c r="F86" s="22" t="n"/>
       <c r="G86" s="22" t="n"/>
       <c r="H86" s="11" t="n"/>
-      <c r="I86" s="27" t="inlineStr">
+      <c r="I86" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J86" s="84" t="n"/>
-      <c r="K86" s="80" t="inlineStr">
+      <c r="J86" s="27" t="n"/>
+      <c r="K86" s="32" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M86" s="36" t="n"/>
-      <c r="N86" s="94" t="n"/>
+      <c r="M86" s="34" t="n"/>
+      <c r="N86" s="98" t="n"/>
     </row>
     <row r="87" ht="15" customHeight="1" thickBot="1">
       <c r="C87" s="4" t="n"/>
@@ -3113,13 +3129,13 @@
       <c r="F87" s="22" t="n"/>
       <c r="G87" s="22" t="n"/>
       <c r="H87" s="11" t="n"/>
-      <c r="I87" s="40" t="inlineStr">
+      <c r="I87" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J87" s="100" t="n"/>
-      <c r="N87" s="94" t="n"/>
+      <c r="J87" s="104" t="n"/>
+      <c r="N87" s="98" t="n"/>
     </row>
     <row r="88">
       <c r="C88" s="4" t="n"/>
@@ -3128,19 +3144,19 @@
       <c r="F88" s="22" t="n"/>
       <c r="G88" s="22" t="n"/>
       <c r="H88" s="11" t="n"/>
-      <c r="I88" s="33" t="inlineStr">
+      <c r="I88" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J88" s="16" t="n"/>
-      <c r="K88" s="26" t="inlineStr">
+      <c r="K88" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M88" s="29" t="n"/>
-      <c r="N88" s="94" t="n"/>
+      <c r="M88" s="38" t="n"/>
+      <c r="N88" s="98" t="n"/>
     </row>
     <row r="89">
       <c r="C89" s="4" t="n"/>
@@ -3149,14 +3165,14 @@
       <c r="F89" s="22" t="n"/>
       <c r="G89" s="22" t="n"/>
       <c r="H89" s="11" t="n"/>
-      <c r="I89" s="80" t="inlineStr">
+      <c r="I89" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J89" s="82" t="n"/>
-      <c r="K89" s="92" t="n"/>
-      <c r="N89" s="94" t="n"/>
+      <c r="J89" s="37" t="n"/>
+      <c r="K89" s="96" t="n"/>
+      <c r="N89" s="98" t="n"/>
     </row>
     <row r="90">
       <c r="C90" s="4" t="n"/>
@@ -3165,19 +3181,19 @@
       <c r="F90" s="22" t="n"/>
       <c r="G90" s="22" t="n"/>
       <c r="H90" s="11" t="n"/>
-      <c r="I90" s="80" t="inlineStr">
+      <c r="I90" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J90" s="14" t="n"/>
-      <c r="K90" s="27" t="inlineStr">
+      <c r="K90" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M90" s="31" t="n"/>
-      <c r="N90" s="94" t="n"/>
+      <c r="M90" s="42" t="n"/>
+      <c r="N90" s="98" t="n"/>
     </row>
     <row r="91" ht="15" customHeight="1" thickBot="1">
       <c r="C91" s="5" t="n"/>
@@ -3186,25 +3202,25 @@
       <c r="F91" s="23" t="n"/>
       <c r="G91" s="23" t="n"/>
       <c r="H91" s="25" t="n"/>
-      <c r="I91" s="28" t="inlineStr">
+      <c r="I91" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J91" s="17" t="n"/>
-      <c r="K91" s="101" t="n"/>
-      <c r="L91" s="102" t="n"/>
-      <c r="M91" s="102" t="n"/>
-      <c r="N91" s="84" t="n"/>
+      <c r="K91" s="105" t="n"/>
+      <c r="L91" s="106" t="n"/>
+      <c r="M91" s="106" t="n"/>
+      <c r="N91" s="27" t="n"/>
     </row>
     <row r="92" ht="15" customHeight="1" thickBot="1">
-      <c r="C92" s="37" t="inlineStr">
+      <c r="C92" s="43" t="inlineStr">
         <is>
           <t>Catcher's View</t>
         </is>
       </c>
-      <c r="D92" s="85" t="n"/>
-      <c r="E92" s="86" t="n"/>
+      <c r="D92" s="89" t="n"/>
+      <c r="E92" s="90" t="n"/>
       <c r="F92" s="20" t="inlineStr">
         <is>
           <t>Pitch</t>
@@ -3220,20 +3236,20 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="I92" s="42" t="inlineStr">
+      <c r="I92" s="28" t="inlineStr">
         <is>
           <t>Situation</t>
         </is>
       </c>
-      <c r="J92" s="86" t="n"/>
-      <c r="K92" s="42" t="inlineStr">
+      <c r="J92" s="90" t="n"/>
+      <c r="K92" s="28" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="L92" s="85" t="n"/>
-      <c r="M92" s="85" t="n"/>
-      <c r="N92" s="86" t="n"/>
+      <c r="L92" s="89" t="n"/>
+      <c r="M92" s="89" t="n"/>
+      <c r="N92" s="90" t="n"/>
     </row>
     <row r="93" ht="14.5" customHeight="1">
       <c r="C93" s="2" t="n"/>
@@ -3242,20 +3258,20 @@
       <c r="F93" s="21" t="n"/>
       <c r="G93" s="21" t="n"/>
       <c r="H93" s="10" t="n"/>
-      <c r="I93" s="32" t="inlineStr">
+      <c r="I93" s="84" t="inlineStr">
         <is>
           <t>Inning:</t>
         </is>
       </c>
-      <c r="J93" s="83" t="n"/>
-      <c r="K93" s="32" t="inlineStr">
+      <c r="J93" s="26" t="n"/>
+      <c r="K93" s="84" t="inlineStr">
         <is>
           <t>Exit Velo:</t>
         </is>
       </c>
-      <c r="L93" s="85" t="n"/>
-      <c r="M93" s="35" t="n"/>
-      <c r="N93" s="88" t="n"/>
+      <c r="L93" s="89" t="n"/>
+      <c r="M93" s="48" t="n"/>
+      <c r="N93" s="92" t="n"/>
     </row>
     <row r="94">
       <c r="C94" s="4" t="n"/>
@@ -3264,14 +3280,14 @@
       <c r="F94" s="22" t="n"/>
       <c r="G94" s="22" t="n"/>
       <c r="H94" s="11" t="n"/>
-      <c r="I94" s="26" t="inlineStr">
+      <c r="I94" s="31" t="inlineStr">
         <is>
           <t>Outs:</t>
         </is>
       </c>
-      <c r="J94" s="29" t="n"/>
-      <c r="K94" s="92" t="n"/>
-      <c r="N94" s="94" t="n"/>
+      <c r="J94" s="38" t="n"/>
+      <c r="K94" s="96" t="n"/>
+      <c r="N94" s="98" t="n"/>
     </row>
     <row r="95">
       <c r="C95" s="4" t="n"/>
@@ -3280,19 +3296,19 @@
       <c r="F95" s="22" t="n"/>
       <c r="G95" s="22" t="n"/>
       <c r="H95" s="11" t="n"/>
-      <c r="I95" s="26" t="inlineStr">
+      <c r="I95" s="31" t="inlineStr">
         <is>
           <t>Home:</t>
         </is>
       </c>
-      <c r="J95" s="29" t="n"/>
-      <c r="K95" s="26" t="inlineStr">
+      <c r="J95" s="38" t="n"/>
+      <c r="K95" s="31" t="inlineStr">
         <is>
           <t>Launch Angle:</t>
         </is>
       </c>
-      <c r="M95" s="36" t="n"/>
-      <c r="N95" s="94" t="n"/>
+      <c r="M95" s="34" t="n"/>
+      <c r="N95" s="98" t="n"/>
     </row>
     <row r="96">
       <c r="C96" s="4" t="n"/>
@@ -3301,14 +3317,14 @@
       <c r="F96" s="22" t="n"/>
       <c r="G96" s="22" t="n"/>
       <c r="H96" s="11" t="n"/>
-      <c r="I96" s="26" t="inlineStr">
+      <c r="I96" s="31" t="inlineStr">
         <is>
           <t>Away:</t>
         </is>
       </c>
-      <c r="J96" s="29" t="n"/>
-      <c r="K96" s="92" t="n"/>
-      <c r="N96" s="94" t="n"/>
+      <c r="J96" s="38" t="n"/>
+      <c r="K96" s="96" t="n"/>
+      <c r="N96" s="98" t="n"/>
     </row>
     <row r="97" ht="15" customHeight="1" thickBot="1">
       <c r="C97" s="4" t="n"/>
@@ -3317,19 +3333,19 @@
       <c r="F97" s="22" t="n"/>
       <c r="G97" s="22" t="n"/>
       <c r="H97" s="11" t="n"/>
-      <c r="I97" s="27" t="inlineStr">
+      <c r="I97" s="39" t="inlineStr">
         <is>
           <t>Runners:</t>
         </is>
       </c>
-      <c r="J97" s="84" t="n"/>
-      <c r="K97" s="26" t="inlineStr">
+      <c r="J97" s="27" t="n"/>
+      <c r="K97" s="31" t="inlineStr">
         <is>
           <t>Hit Type:</t>
         </is>
       </c>
-      <c r="M97" s="36" t="n"/>
-      <c r="N97" s="94" t="n"/>
+      <c r="M97" s="34" t="n"/>
+      <c r="N97" s="98" t="n"/>
     </row>
     <row r="98" ht="15" customHeight="1" thickBot="1">
       <c r="C98" s="4" t="n"/>
@@ -3338,14 +3354,14 @@
       <c r="F98" s="22" t="n"/>
       <c r="G98" s="22" t="n"/>
       <c r="H98" s="11" t="n"/>
-      <c r="I98" s="40" t="inlineStr">
+      <c r="I98" s="35" t="inlineStr">
         <is>
           <t>Pitcher Info</t>
         </is>
       </c>
-      <c r="J98" s="100" t="n"/>
-      <c r="K98" s="92" t="n"/>
-      <c r="N98" s="94" t="n"/>
+      <c r="J98" s="104" t="n"/>
+      <c r="K98" s="96" t="n"/>
+      <c r="N98" s="98" t="n"/>
     </row>
     <row r="99">
       <c r="C99" s="4" t="n"/>
@@ -3354,19 +3370,19 @@
       <c r="F99" s="22" t="n"/>
       <c r="G99" s="22" t="n"/>
       <c r="H99" s="11" t="n"/>
-      <c r="I99" s="33" t="inlineStr">
+      <c r="I99" s="46" t="inlineStr">
         <is>
           <t>Name:</t>
         </is>
       </c>
       <c r="J99" s="16" t="n"/>
-      <c r="K99" s="26" t="inlineStr">
+      <c r="K99" s="31" t="inlineStr">
         <is>
           <t>Result:</t>
         </is>
       </c>
-      <c r="M99" s="29" t="n"/>
-      <c r="N99" s="94" t="n"/>
+      <c r="M99" s="38" t="n"/>
+      <c r="N99" s="98" t="n"/>
     </row>
     <row r="100">
       <c r="C100" s="4" t="n"/>
@@ -3375,14 +3391,14 @@
       <c r="F100" s="22" t="n"/>
       <c r="G100" s="22" t="n"/>
       <c r="H100" s="11" t="n"/>
-      <c r="I100" s="80" t="inlineStr">
+      <c r="I100" s="32" t="inlineStr">
         <is>
           <t>Throws:</t>
         </is>
       </c>
-      <c r="J100" s="82" t="n"/>
-      <c r="K100" s="92" t="n"/>
-      <c r="N100" s="94" t="n"/>
+      <c r="J100" s="37" t="n"/>
+      <c r="K100" s="96" t="n"/>
+      <c r="N100" s="98" t="n"/>
     </row>
     <row r="101">
       <c r="C101" s="4" t="n"/>
@@ -3391,19 +3407,19 @@
       <c r="F101" s="22" t="n"/>
       <c r="G101" s="22" t="n"/>
       <c r="H101" s="11" t="n"/>
-      <c r="I101" s="80" t="inlineStr">
+      <c r="I101" s="32" t="inlineStr">
         <is>
           <t>FB Velo:</t>
         </is>
       </c>
       <c r="J101" s="14" t="n"/>
-      <c r="K101" s="27" t="inlineStr">
+      <c r="K101" s="39" t="inlineStr">
         <is>
           <t>QAB:</t>
         </is>
       </c>
-      <c r="M101" s="31" t="n"/>
-      <c r="N101" s="94" t="n"/>
+      <c r="M101" s="42" t="n"/>
+      <c r="N101" s="98" t="n"/>
     </row>
     <row r="102" ht="15" customHeight="1" thickBot="1">
       <c r="C102" s="5" t="n"/>
@@ -3412,52 +3428,95 @@
       <c r="F102" s="23" t="n"/>
       <c r="G102" s="23" t="n"/>
       <c r="H102" s="25" t="n"/>
-      <c r="I102" s="28" t="inlineStr">
+      <c r="I102" s="40" t="inlineStr">
         <is>
           <t>Pitch Mix:</t>
         </is>
       </c>
       <c r="J102" s="17" t="n"/>
-      <c r="K102" s="101" t="n"/>
-      <c r="L102" s="102" t="n"/>
-      <c r="M102" s="102" t="n"/>
-      <c r="N102" s="84" t="n"/>
+      <c r="K102" s="105" t="n"/>
+      <c r="L102" s="106" t="n"/>
+      <c r="M102" s="106" t="n"/>
+      <c r="N102" s="27" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K95:L96"/>
-    <mergeCell ref="M95:N96"/>
-    <mergeCell ref="K97:L98"/>
-    <mergeCell ref="M97:N98"/>
-    <mergeCell ref="I98:J98"/>
-    <mergeCell ref="K99:L100"/>
-    <mergeCell ref="M99:N100"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="K68:L69"/>
-    <mergeCell ref="M68:N69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="K73:L74"/>
-    <mergeCell ref="M73:N74"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="K45:L46"/>
-    <mergeCell ref="M45:N46"/>
-    <mergeCell ref="K47:L48"/>
-    <mergeCell ref="M47:N48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K49:L50"/>
-    <mergeCell ref="M49:N50"/>
-    <mergeCell ref="K51:L52"/>
-    <mergeCell ref="M51:N52"/>
-    <mergeCell ref="K66:L67"/>
-    <mergeCell ref="M66:N67"/>
-    <mergeCell ref="K75:L76"/>
-    <mergeCell ref="M75:N76"/>
-    <mergeCell ref="K64:L65"/>
-    <mergeCell ref="M64:N65"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="K101:L102"/>
+    <mergeCell ref="M101:N102"/>
+    <mergeCell ref="K84:L85"/>
+    <mergeCell ref="M84:N85"/>
+    <mergeCell ref="K93:L94"/>
+    <mergeCell ref="M93:N94"/>
+    <mergeCell ref="K86:L87"/>
+    <mergeCell ref="M86:N87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K88:L89"/>
+    <mergeCell ref="M88:N89"/>
+    <mergeCell ref="K90:L91"/>
+    <mergeCell ref="M90:N91"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="K60:L61"/>
+    <mergeCell ref="M60:N61"/>
+    <mergeCell ref="K62:L63"/>
+    <mergeCell ref="M62:N63"/>
+    <mergeCell ref="K71:L72"/>
+    <mergeCell ref="M71:N72"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K18:L19"/>
+    <mergeCell ref="M18:N19"/>
+    <mergeCell ref="K27:L28"/>
+    <mergeCell ref="M27:N28"/>
+    <mergeCell ref="K21:L22"/>
+    <mergeCell ref="M21:N22"/>
+    <mergeCell ref="K23:L24"/>
+    <mergeCell ref="M23:N24"/>
+    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="K12:L13"/>
+    <mergeCell ref="M14:N15"/>
+    <mergeCell ref="M10:N11"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K14:L15"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="M12:N13"/>
+    <mergeCell ref="M16:N17"/>
+    <mergeCell ref="M3:N8"/>
+    <mergeCell ref="C3:E4"/>
+    <mergeCell ref="C5:E6"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F3:L5"/>
+    <mergeCell ref="F6:L8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="M38:N39"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M40:N41"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:L44"/>
+    <mergeCell ref="M43:N44"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K36:L37"/>
+    <mergeCell ref="M36:N37"/>
+    <mergeCell ref="K25:L26"/>
+    <mergeCell ref="M25:N26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K29:L30"/>
+    <mergeCell ref="M29:N30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K34:L35"/>
+    <mergeCell ref="M34:N35"/>
     <mergeCell ref="K77:L78"/>
     <mergeCell ref="M77:N78"/>
     <mergeCell ref="K79:L80"/>
@@ -3471,84 +3530,41 @@
     <mergeCell ref="C55:E56"/>
     <mergeCell ref="F56:L58"/>
     <mergeCell ref="C57:E58"/>
-    <mergeCell ref="K25:L26"/>
-    <mergeCell ref="M25:N26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K29:L30"/>
-    <mergeCell ref="M29:N30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K34:L35"/>
-    <mergeCell ref="M34:N35"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="M38:N39"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="M40:N41"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:L44"/>
-    <mergeCell ref="M43:N44"/>
-    <mergeCell ref="M3:N8"/>
-    <mergeCell ref="C3:E4"/>
-    <mergeCell ref="C5:E6"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F3:L5"/>
-    <mergeCell ref="F6:L8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:L11"/>
-    <mergeCell ref="K12:L13"/>
-    <mergeCell ref="M14:N15"/>
-    <mergeCell ref="M10:N11"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K14:L15"/>
-    <mergeCell ref="K16:L17"/>
-    <mergeCell ref="M12:N13"/>
-    <mergeCell ref="M16:N17"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K18:L19"/>
-    <mergeCell ref="M18:N19"/>
-    <mergeCell ref="K27:L28"/>
-    <mergeCell ref="M27:N28"/>
-    <mergeCell ref="K21:L22"/>
-    <mergeCell ref="M21:N22"/>
-    <mergeCell ref="K23:L24"/>
-    <mergeCell ref="M23:N24"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K36:L37"/>
-    <mergeCell ref="M36:N37"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="K60:L61"/>
-    <mergeCell ref="M60:N61"/>
-    <mergeCell ref="K62:L63"/>
-    <mergeCell ref="M62:N63"/>
-    <mergeCell ref="K71:L72"/>
-    <mergeCell ref="M71:N72"/>
     <mergeCell ref="I81:J81"/>
     <mergeCell ref="C81:E81"/>
-    <mergeCell ref="K84:L85"/>
-    <mergeCell ref="M84:N85"/>
-    <mergeCell ref="K93:L94"/>
-    <mergeCell ref="M93:N94"/>
-    <mergeCell ref="K86:L87"/>
-    <mergeCell ref="M86:N87"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="K88:L89"/>
-    <mergeCell ref="M88:N89"/>
-    <mergeCell ref="K90:L91"/>
-    <mergeCell ref="M90:N91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="K101:L102"/>
-    <mergeCell ref="M101:N102"/>
+    <mergeCell ref="K45:L46"/>
+    <mergeCell ref="M45:N46"/>
+    <mergeCell ref="K47:L48"/>
+    <mergeCell ref="M47:N48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K49:L50"/>
+    <mergeCell ref="M49:N50"/>
+    <mergeCell ref="K51:L52"/>
+    <mergeCell ref="M51:N52"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K68:L69"/>
+    <mergeCell ref="M68:N69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="K73:L74"/>
+    <mergeCell ref="M73:N74"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="K66:L67"/>
+    <mergeCell ref="M66:N67"/>
+    <mergeCell ref="K75:L76"/>
+    <mergeCell ref="M75:N76"/>
+    <mergeCell ref="K64:L65"/>
+    <mergeCell ref="M64:N65"/>
+    <mergeCell ref="I92:J92"/>
+    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="K95:L96"/>
+    <mergeCell ref="M95:N96"/>
+    <mergeCell ref="K97:L98"/>
+    <mergeCell ref="M97:N98"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="K99:L100"/>
+    <mergeCell ref="M99:N100"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
just need to make chart for pitcher report
</commit_message>
<xml_diff>
--- a/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
+++ b/postgame_hitter_reports/COR_KNI/2022-07-29/Advincula, Jonah.xlsx
@@ -1667,7 +1667,7 @@
       </c>
       <c r="J19" s="17" t="inlineStr">
         <is>
-          <t>CH,FB,SL</t>
+          <t>CH,SL,FB</t>
         </is>
       </c>
       <c r="K19" s="105" t="n"/>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="J30" s="17" t="inlineStr">
         <is>
-          <t>CH,FB,SL</t>
+          <t>CH,SL,FB</t>
         </is>
       </c>
       <c r="K30" s="105" t="n"/>

</xml_diff>